<commit_message>
Preproducción antes del Hardening versión funcional previa.
</commit_message>
<xml_diff>
--- a/Gastos Socios Symbiot.xlsx
+++ b/Gastos Socios Symbiot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\symbiot\symbiot_finance_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9EECBC-ED61-4267-AFD9-1148193742B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB88F87-CCEC-4994-BEBA-42DAF7CA20D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" tabRatio="773" activeTab="2" xr2:uid="{9089598D-A971-4695-A3E9-38E00D99589C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" tabRatio="773" activeTab="1" xr2:uid="{9089598D-A971-4695-A3E9-38E00D99589C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingresos Symbiot" sheetId="11" r:id="rId1"/>
@@ -2880,27 +2880,6 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0;[Red]#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
@@ -2941,6 +2920,27 @@
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="#,##0;[Red]#,##0"/>
     </dxf>
     <dxf>
       <font>
@@ -18032,6 +18032,681 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B8A3BFAB-FC5E-43A6-8CF5-E0F2F569B261}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A61:D71" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item m="1" x="11"/>
+        <item m="1" x="10"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="8"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="15" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Suma de Noviembre3" fld="45" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="20">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0FFE308-1BD4-44FF-A072-2E4430C91117}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A75:D82" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="8"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="15" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Alumno" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="24">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="23">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="2" selected="0">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36B00CA7-DB1E-4E6F-A153-B286F31CD045}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A47:D57" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item m="1" x="11"/>
+        <item m="1" x="10"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Estatus" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="15" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E247F413-26A1-461C-B7BB-658F3FD47111}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A21:D31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="13">
+        <item m="1" x="11"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item m="1" x="10"/>
+        <item m="1" x="9"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item h="1" x="0"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="8"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="15" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Alumno" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="32">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="7">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="29">
+      <pivotArea field="8" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7FBE22C9-837E-4438-83F0-A08643171F67}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="49">
@@ -18184,17 +18859,17 @@
     <dataField name="Sum of Total" fld="47" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="19">
+    <format dxfId="35">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="34">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
@@ -18214,7 +18889,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E9EF0DE-BAA0-4B82-BC94-4C4F1D62E987}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A35:D42" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
@@ -18336,13 +19011,13 @@
     <dataField name="Suma de Noviembre3" fld="45" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="23">
+    <format dxfId="39">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="38">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="37">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2" selected="0">
@@ -18352,7 +19027,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2">
@@ -18361,681 +19036,6 @@
           </reference>
         </references>
       </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B8A3BFAB-FC5E-43A6-8CF5-E0F2F569B261}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A61:D71" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item m="1" x="11"/>
-        <item m="1" x="10"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="8"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="15" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Suma de Noviembre3" fld="45" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="27">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="26">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="25">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="2" selected="0">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0FFE308-1BD4-44FF-A072-2E4430C91117}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A75:D82" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="8"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="15" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Alumno" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="31">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="30">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="29">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="2" selected="0">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="28">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36B00CA7-DB1E-4E6F-A153-B286F31CD045}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A47:D57" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item m="1" x="11"/>
-        <item m="1" x="10"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item h="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Estatus" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="34">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="33">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="15" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E247F413-26A1-461C-B7BB-658F3FD47111}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A21:D31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item m="1" x="11"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item m="1" x="10"/>
-        <item m="1" x="9"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item h="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item h="1" x="0"/>
-        <item h="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="8"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="15" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Alumno" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="5">
-    <format dxfId="39">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="7">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="36">
-      <pivotArea field="8" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0" selected="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -20346,7 +20346,13 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}" name="Table1" displayName="Table1" ref="A1:H737" totalsRowCount="1" headerRowDxfId="50">
-  <autoFilter ref="A1:H736" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}"/>
+  <autoFilter ref="A1:H736" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Escuela"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H736">
     <sortCondition ref="A1:A736"/>
   </sortState>
@@ -20879,7 +20885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0DCBCA-5B69-43D6-9082-970D5445E651}">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -22413,11 +22419,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494CB971-7A44-471B-94F3-86880B27AB17}">
   <dimension ref="A1:AY120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="H89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J84" sqref="J84"/>
+      <selection pane="bottomRight" activeCell="AS11" sqref="AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23050,7 +23056,9 @@
       <c r="AT4" s="30">
         <v>0</v>
       </c>
-      <c r="AU4" s="23"/>
+      <c r="AU4" s="30">
+        <v>0</v>
+      </c>
       <c r="AV4" s="38">
         <f>SUM(Table14[[#This Row],[Julio]:[Diciembre2]])</f>
         <v>3825</v>
@@ -24955,7 +24963,9 @@
       <c r="AT17" s="30">
         <v>0</v>
       </c>
-      <c r="AU17" s="30"/>
+      <c r="AU17" s="30">
+        <v>0</v>
+      </c>
       <c r="AV17" s="63">
         <f>SUM(Table14[[#This Row],[Julio]:[Diciembre2]])</f>
         <v>5100</v>
@@ -38861,8 +38871,8 @@
   <dimension ref="A1:L737"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A703" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D721" sqref="D721"/>
+      <pane ySplit="1" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -38904,7 +38914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>45016</v>
       </c>
@@ -38931,7 +38941,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>45016</v>
       </c>
@@ -38958,7 +38968,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>45051</v>
       </c>
@@ -38985,7 +38995,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>45059</v>
       </c>
@@ -39012,7 +39022,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>45059</v>
       </c>
@@ -39039,7 +39049,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>45063</v>
       </c>
@@ -39066,7 +39076,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>45063</v>
       </c>
@@ -39093,7 +39103,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>45063</v>
       </c>
@@ -39120,7 +39130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>45068</v>
       </c>
@@ -39147,7 +39157,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>45069</v>
       </c>
@@ -39174,7 +39184,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>45069</v>
       </c>
@@ -39201,7 +39211,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>45069</v>
       </c>
@@ -39228,7 +39238,7 @@
         <v>953.16000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>45069</v>
       </c>
@@ -39255,7 +39265,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>45069</v>
       </c>
@@ -39282,7 +39292,7 @@
         <v>287.96999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>45076</v>
       </c>
@@ -39309,7 +39319,7 @@
         <v>8250</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>45076</v>
       </c>
@@ -39336,7 +39346,7 @@
         <v>13419</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>45076</v>
       </c>
@@ -39363,7 +39373,7 @@
         <v>15196</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>45076</v>
       </c>
@@ -39390,7 +39400,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>45076</v>
       </c>
@@ -39416,7 +39426,7 @@
         <v>15198</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>45077</v>
       </c>
@@ -39443,7 +39453,7 @@
         <v>2427</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>45077</v>
       </c>
@@ -39470,7 +39480,7 @@
         <v>880.44</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>45077</v>
       </c>
@@ -39497,7 +39507,7 @@
         <v>3284.49</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>45077</v>
       </c>
@@ -39524,7 +39534,7 @@
         <v>406.89</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>45077</v>
       </c>
@@ -39551,7 +39561,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>45077</v>
       </c>
@@ -39578,7 +39588,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>45077</v>
       </c>
@@ -39605,7 +39615,7 @@
         <v>5697</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>45079</v>
       </c>
@@ -39632,7 +39642,7 @@
         <v>2994</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>45079</v>
       </c>
@@ -39659,7 +39669,7 @@
         <v>14.67</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>45079</v>
       </c>
@@ -39686,7 +39696,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>45079</v>
       </c>
@@ -39713,7 +39723,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>45079</v>
       </c>
@@ -39740,7 +39750,7 @@
         <v>4395</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>45079</v>
       </c>
@@ -39767,7 +39777,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>45079</v>
       </c>
@@ -39794,7 +39804,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>45079</v>
       </c>
@@ -39821,7 +39831,7 @@
         <v>3675</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>45081</v>
       </c>
@@ -39848,7 +39858,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>45083</v>
       </c>
@@ -39875,7 +39885,7 @@
         <v>1105.9499999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>45083</v>
       </c>
@@ -39902,7 +39912,7 @@
         <v>1330.29</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>45083</v>
       </c>
@@ -39929,7 +39939,7 @@
         <v>10468</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>45088</v>
       </c>
@@ -39956,7 +39966,7 @@
         <v>1928.64</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>45091</v>
       </c>
@@ -39983,7 +39993,7 @@
         <v>21942.34</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>45092</v>
       </c>
@@ -40010,7 +40020,7 @@
         <v>7621</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>45093</v>
       </c>
@@ -40037,7 +40047,7 @@
         <v>778.05</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>45094</v>
       </c>
@@ -40064,7 +40074,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>45095</v>
       </c>
@@ -40091,7 +40101,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45096</v>
       </c>
@@ -40118,7 +40128,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>45097</v>
       </c>
@@ -40145,7 +40155,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>45098</v>
       </c>
@@ -40172,7 +40182,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>45100</v>
       </c>
@@ -40199,7 +40209,7 @@
         <v>8224.8799999999992</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>45100</v>
       </c>
@@ -40226,7 +40236,7 @@
         <v>-8224.8799999999992</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3">
         <v>45100</v>
       </c>
@@ -40253,7 +40263,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3">
         <v>45100</v>
       </c>
@@ -40280,7 +40290,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3">
         <v>45100</v>
       </c>
@@ -40307,7 +40317,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3">
         <v>45100</v>
       </c>
@@ -40334,7 +40344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3">
         <v>45100</v>
       </c>
@@ -40361,7 +40371,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3">
         <v>45100</v>
       </c>
@@ -40388,7 +40398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3">
         <v>45100</v>
       </c>
@@ -40415,7 +40425,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3">
         <v>45100</v>
       </c>
@@ -40442,7 +40452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3">
         <v>45100</v>
       </c>
@@ -40469,7 +40479,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3">
         <v>45100</v>
       </c>
@@ -40496,7 +40506,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3">
         <v>45100</v>
       </c>
@@ -40523,7 +40533,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3">
         <v>45100</v>
       </c>
@@ -40550,7 +40560,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3">
         <v>45100</v>
       </c>
@@ -40577,7 +40587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3">
         <v>45100</v>
       </c>
@@ -40604,7 +40614,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3">
         <v>45100</v>
       </c>
@@ -40631,7 +40641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3">
         <v>45100</v>
       </c>
@@ -40658,7 +40668,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3">
         <v>45100</v>
       </c>
@@ -40685,7 +40695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3">
         <v>45100</v>
       </c>
@@ -40712,7 +40722,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3">
         <v>45103</v>
       </c>
@@ -40739,7 +40749,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3">
         <v>45103</v>
       </c>
@@ -40766,7 +40776,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3">
         <v>45107</v>
       </c>
@@ -40793,7 +40803,7 @@
         <v>3550</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3">
         <v>45108</v>
       </c>
@@ -40820,7 +40830,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3">
         <v>45111</v>
       </c>
@@ -40847,7 +40857,7 @@
         <v>2547</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3">
         <v>45111</v>
       </c>
@@ -40874,7 +40884,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3">
         <v>45111</v>
       </c>
@@ -40901,7 +40911,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3">
         <v>45111</v>
       </c>
@@ -40928,7 +40938,7 @@
         <v>3525.35</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3">
         <v>45111</v>
       </c>
@@ -40955,7 +40965,7 @@
         <v>6845</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3">
         <v>45111</v>
       </c>
@@ -40982,7 +40992,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3">
         <v>45111</v>
       </c>
@@ -41009,7 +41019,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3">
         <v>45111</v>
       </c>
@@ -41037,7 +41047,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3">
         <v>45111</v>
       </c>
@@ -41064,7 +41074,7 @@
         <v>3712</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3">
         <v>45113</v>
       </c>
@@ -41091,7 +41101,7 @@
         <v>2813.77</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3">
         <v>45113</v>
       </c>
@@ -41118,7 +41128,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3">
         <v>45114</v>
       </c>
@@ -41145,7 +41155,7 @@
         <v>6800</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3">
         <v>45116</v>
       </c>
@@ -41172,7 +41182,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3">
         <v>45116</v>
       </c>
@@ -41199,7 +41209,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3">
         <v>45118</v>
       </c>
@@ -41226,7 +41236,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3">
         <v>45119</v>
       </c>
@@ -41253,7 +41263,7 @@
         <v>427.24</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3">
         <v>45119</v>
       </c>
@@ -41280,7 +41290,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3">
         <v>45119</v>
       </c>
@@ -41307,7 +41317,7 @@
         <v>317.72000000000003</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3">
         <v>45120</v>
       </c>
@@ -41334,7 +41344,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3">
         <v>45120</v>
       </c>
@@ -41361,7 +41371,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3">
         <v>45120</v>
       </c>
@@ -41388,7 +41398,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3">
         <v>45120</v>
       </c>
@@ -41415,7 +41425,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3">
         <v>45120</v>
       </c>
@@ -41442,7 +41452,7 @@
         <v>3199</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3">
         <v>45120</v>
       </c>
@@ -41469,7 +41479,7 @@
         <v>3499</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3">
         <v>45122</v>
       </c>
@@ -41497,7 +41507,7 @@
         <v>3598</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3">
         <v>45124</v>
       </c>
@@ -41524,7 +41534,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3">
         <v>45124</v>
       </c>
@@ -41551,7 +41561,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3">
         <v>45124</v>
       </c>
@@ -41578,7 +41588,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3">
         <v>45124</v>
       </c>
@@ -41605,7 +41615,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3">
         <v>45124</v>
       </c>
@@ -41632,7 +41642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3">
         <v>45124</v>
       </c>
@@ -41659,7 +41669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3">
         <v>45124</v>
       </c>
@@ -41686,7 +41696,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3">
         <v>45127</v>
       </c>
@@ -41713,7 +41723,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3">
         <v>45128</v>
       </c>
@@ -41740,7 +41750,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3">
         <v>45128</v>
       </c>
@@ -41767,7 +41777,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3">
         <v>45129</v>
       </c>
@@ -41794,7 +41804,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3">
         <v>45129</v>
       </c>
@@ -41821,7 +41831,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3">
         <v>45131</v>
       </c>
@@ -41848,7 +41858,7 @@
         <v>6999</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3">
         <v>45131</v>
       </c>
@@ -41875,7 +41885,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3">
         <v>45131</v>
       </c>
@@ -41902,7 +41912,7 @@
         <v>2766</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3">
         <v>45132</v>
       </c>
@@ -41929,7 +41939,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3">
         <v>45136</v>
       </c>
@@ -41956,7 +41966,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3">
         <v>45136</v>
       </c>
@@ -41983,7 +41993,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3">
         <v>45136</v>
       </c>
@@ -42010,7 +42020,7 @@
         <v>3839</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A117" s="3">
         <v>45138</v>
       </c>
@@ -42038,7 +42048,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A118" s="3">
         <v>45138</v>
       </c>
@@ -42065,7 +42075,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A119" s="3">
         <v>45139</v>
       </c>
@@ -42092,7 +42102,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A120" s="3">
         <v>45139</v>
       </c>
@@ -42119,7 +42129,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A121" s="3">
         <v>45143</v>
       </c>
@@ -42173,7 +42183,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A123" s="3">
         <v>45144</v>
       </c>
@@ -42200,7 +42210,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A124" s="3">
         <v>45150</v>
       </c>
@@ -42227,7 +42237,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A125" s="3">
         <v>45153</v>
       </c>
@@ -42254,7 +42264,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A126" s="3">
         <v>45153</v>
       </c>
@@ -42281,7 +42291,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A127" s="3">
         <v>45153</v>
       </c>
@@ -42308,7 +42318,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A128" s="3">
         <v>45153</v>
       </c>
@@ -42335,7 +42345,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A129" s="3">
         <v>45155</v>
       </c>
@@ -42362,7 +42372,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A130" s="3">
         <v>45155</v>
       </c>
@@ -42389,7 +42399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A131" s="3">
         <v>45157</v>
       </c>
@@ -42416,7 +42426,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A132" s="3">
         <v>45159</v>
       </c>
@@ -42443,7 +42453,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A133" s="3">
         <v>45160</v>
       </c>
@@ -42470,7 +42480,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A134" s="3">
         <v>45160</v>
       </c>
@@ -42497,7 +42507,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A135" s="3">
         <v>45160</v>
       </c>
@@ -42524,7 +42534,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A136" s="3">
         <v>45160</v>
       </c>
@@ -42551,7 +42561,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A137" s="3">
         <v>45161</v>
       </c>
@@ -42578,7 +42588,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A138" s="3">
         <v>45162</v>
       </c>
@@ -42605,7 +42615,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A139" s="3">
         <v>45162</v>
       </c>
@@ -42632,7 +42642,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A140" s="3">
         <v>45164</v>
       </c>
@@ -42686,7 +42696,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A142" s="3">
         <v>45167</v>
       </c>
@@ -42713,7 +42723,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A143" s="3">
         <v>45169</v>
       </c>
@@ -42740,7 +42750,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A144" s="3">
         <v>45169</v>
       </c>
@@ -42794,7 +42804,7 @@
         <v>488.36</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A146" s="3">
         <v>45171</v>
       </c>
@@ -42901,7 +42911,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A150" s="3">
         <v>45178</v>
       </c>
@@ -42928,7 +42938,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A151" s="3">
         <v>45184</v>
       </c>
@@ -42955,7 +42965,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A152" s="3">
         <v>45189</v>
       </c>
@@ -42982,7 +42992,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A153" s="3">
         <v>45190</v>
       </c>
@@ -43009,7 +43019,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A154" s="3">
         <v>45193</v>
       </c>
@@ -43036,7 +43046,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A155" s="3">
         <v>45195</v>
       </c>
@@ -43063,7 +43073,7 @@
         <v>8816</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A156" s="3">
         <v>45199</v>
       </c>
@@ -43090,7 +43100,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A157" s="3">
         <v>45199</v>
       </c>
@@ -43117,7 +43127,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A158" s="3">
         <v>45199</v>
       </c>
@@ -43144,7 +43154,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A159" s="3">
         <v>45199</v>
       </c>
@@ -43171,7 +43181,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A160" s="3">
         <v>45199</v>
       </c>
@@ -43198,7 +43208,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A161" s="3">
         <v>45199</v>
       </c>
@@ -43225,7 +43235,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A162" s="3">
         <v>45199</v>
       </c>
@@ -43279,7 +43289,7 @@
         <v>945.11</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A164" s="3">
         <v>45200</v>
       </c>
@@ -43306,7 +43316,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A165" s="3">
         <v>45200</v>
       </c>
@@ -43333,7 +43343,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A166" s="3">
         <v>45203</v>
       </c>
@@ -43360,7 +43370,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A167" s="3">
         <v>45205</v>
       </c>
@@ -43387,7 +43397,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A168" s="3">
         <v>45206</v>
       </c>
@@ -43414,7 +43424,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A169" s="3">
         <v>45213</v>
       </c>
@@ -43441,7 +43451,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A170" s="3">
         <v>45214</v>
       </c>
@@ -43468,7 +43478,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A171" s="3">
         <v>45215</v>
       </c>
@@ -43495,7 +43505,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A172" s="3">
         <v>45219</v>
       </c>
@@ -43522,7 +43532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A173" s="3">
         <v>45219</v>
       </c>
@@ -43549,7 +43559,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A174" s="3">
         <v>45220</v>
       </c>
@@ -43576,7 +43586,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A175" s="3">
         <v>45227</v>
       </c>
@@ -43603,7 +43613,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A176" s="3">
         <v>45230</v>
       </c>
@@ -43630,7 +43640,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A177" s="3">
         <v>45230</v>
       </c>
@@ -43657,7 +43667,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A178" s="3">
         <v>45230</v>
       </c>
@@ -43684,7 +43694,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A179" s="3">
         <v>45230</v>
       </c>
@@ -43765,7 +43775,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A182" s="3">
         <v>45230</v>
       </c>
@@ -43792,7 +43802,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A183" s="3">
         <v>45230</v>
       </c>
@@ -43819,7 +43829,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A184" s="3">
         <v>45230</v>
       </c>
@@ -43846,7 +43856,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A185" s="3">
         <v>45230</v>
       </c>
@@ -43873,7 +43883,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A186" s="3">
         <v>45230</v>
       </c>
@@ -43900,7 +43910,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A187" s="3">
         <v>45230</v>
       </c>
@@ -43927,7 +43937,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A188" s="3">
         <v>45230</v>
       </c>
@@ -43954,7 +43964,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A189" s="3">
         <v>45234</v>
       </c>
@@ -43981,7 +43991,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A190" s="3">
         <v>45240</v>
       </c>
@@ -44008,7 +44018,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A191" s="3">
         <v>45242</v>
       </c>
@@ -44035,7 +44045,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A192" s="3">
         <v>45244</v>
       </c>
@@ -44062,7 +44072,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A193" s="3">
         <v>45246</v>
       </c>
@@ -44116,7 +44126,7 @@
         <v>4408</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A195" s="3">
         <v>45248</v>
       </c>
@@ -44143,7 +44153,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A196" s="3">
         <v>45250</v>
       </c>
@@ -44278,7 +44288,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A201" s="3">
         <v>45260</v>
       </c>
@@ -44332,7 +44342,7 @@
         <v>800.98</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A203" s="3">
         <v>45260</v>
       </c>
@@ -44359,7 +44369,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A204" s="3">
         <v>45260</v>
       </c>
@@ -44386,7 +44396,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A205" s="3">
         <v>45260</v>
       </c>
@@ -44413,7 +44423,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A206" s="3">
         <v>45260</v>
       </c>
@@ -44440,7 +44450,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A207" s="3">
         <v>45260</v>
       </c>
@@ -44467,7 +44477,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A208" s="3">
         <v>45262</v>
       </c>
@@ -44494,7 +44504,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A209" s="3">
         <v>45269</v>
       </c>
@@ -44548,7 +44558,7 @@
         <v>349.12</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A211" s="3">
         <v>45276</v>
       </c>
@@ -44575,7 +44585,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A212" s="3">
         <v>45276</v>
       </c>
@@ -44602,7 +44612,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A213" s="3">
         <v>45276</v>
       </c>
@@ -44629,7 +44639,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A214" s="3">
         <v>45278</v>
       </c>
@@ -44684,7 +44694,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A216" s="3">
         <v>45281</v>
       </c>
@@ -44711,7 +44721,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A217" s="3">
         <v>45281</v>
       </c>
@@ -44792,7 +44802,7 @@
         <v>813.16</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A220" s="3">
         <v>45291</v>
       </c>
@@ -44819,7 +44829,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A221" s="3">
         <v>45291</v>
       </c>
@@ -44846,7 +44856,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A222" s="3">
         <v>45291</v>
       </c>
@@ -44873,7 +44883,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A223" s="3">
         <v>45291</v>
       </c>
@@ -44900,7 +44910,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.4">
       <c r="A224" s="3">
         <v>45291</v>
       </c>
@@ -44927,7 +44937,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A225" s="3">
         <v>45296</v>
       </c>
@@ -44981,7 +44991,7 @@
         <v>4486</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A227" s="3">
         <v>45297</v>
       </c>
@@ -45008,7 +45018,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A228" s="3">
         <v>45298</v>
       </c>
@@ -45089,7 +45099,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A231" s="3">
         <v>45306</v>
       </c>
@@ -45143,7 +45153,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A233" s="3">
         <v>45307</v>
       </c>
@@ -45197,7 +45207,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A235" s="3">
         <v>45313</v>
       </c>
@@ -45224,7 +45234,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A236" s="3">
         <v>45313</v>
       </c>
@@ -45251,7 +45261,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A237" s="3">
         <v>45313</v>
       </c>
@@ -45278,7 +45288,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A238" s="3">
         <v>45320</v>
       </c>
@@ -45332,7 +45342,7 @@
         <v>813.16</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A240" s="3">
         <v>45322</v>
       </c>
@@ -45359,7 +45369,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A241" s="3">
         <v>45322</v>
       </c>
@@ -45386,7 +45396,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A242" s="3">
         <v>45322</v>
       </c>
@@ -45413,7 +45423,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A243" s="3">
         <v>45322</v>
       </c>
@@ -45440,7 +45450,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A244" s="3">
         <v>45322</v>
       </c>
@@ -45467,7 +45477,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A245" s="3">
         <v>45324</v>
       </c>
@@ -45494,7 +45504,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A246" s="3">
         <v>45324</v>
       </c>
@@ -45521,7 +45531,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A247" s="3">
         <v>45325</v>
       </c>
@@ -45548,7 +45558,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A248" s="3">
         <v>45325</v>
       </c>
@@ -45656,7 +45666,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A252" s="3">
         <v>45325</v>
       </c>
@@ -45737,7 +45747,7 @@
         <v>343.42</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A255" s="3">
         <v>45338</v>
       </c>
@@ -45764,7 +45774,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A256" s="3">
         <v>45340</v>
       </c>
@@ -45818,7 +45828,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A258" s="3">
         <v>45345</v>
       </c>
@@ -45845,7 +45855,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A259" s="3">
         <v>45345</v>
       </c>
@@ -45926,7 +45936,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A262" s="3">
         <v>45350</v>
       </c>
@@ -45980,7 +45990,7 @@
         <v>752.26</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A264" s="3">
         <v>45351</v>
       </c>
@@ -46115,7 +46125,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A269" s="3">
         <v>45353</v>
       </c>
@@ -46223,7 +46233,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A273" s="3">
         <v>45363</v>
       </c>
@@ -46385,7 +46395,7 @@
         <v>11560</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A279" s="3">
         <v>45376</v>
       </c>
@@ -46466,7 +46476,7 @@
         <v>949.17</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A282" s="3">
         <v>45382</v>
       </c>
@@ -46601,7 +46611,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A287" s="3">
         <v>45386</v>
       </c>
@@ -46737,7 +46747,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A292" s="3">
         <v>45399</v>
       </c>
@@ -46791,7 +46801,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A294" s="3">
         <v>45403</v>
       </c>
@@ -46818,7 +46828,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A295" s="3">
         <v>45403</v>
       </c>
@@ -46899,7 +46909,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A298" s="3">
         <v>45411</v>
       </c>
@@ -46926,7 +46936,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A299" s="3">
         <v>45412</v>
       </c>
@@ -46953,7 +46963,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A300" s="3">
         <v>45412</v>
       </c>
@@ -46980,7 +46990,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A301" s="3">
         <v>45412</v>
       </c>
@@ -47007,7 +47017,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A302" s="3">
         <v>45412</v>
       </c>
@@ -47061,7 +47071,7 @@
         <v>711.66</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A304" s="3">
         <v>45416</v>
       </c>
@@ -47088,7 +47098,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A305" s="3">
         <v>45416</v>
       </c>
@@ -47169,7 +47179,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A308" s="3">
         <v>45420</v>
       </c>
@@ -47196,7 +47206,7 @@
         <v>-5000</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A309" s="3">
         <v>45420</v>
       </c>
@@ -47277,7 +47287,7 @@
         <v>3659</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A312" s="3">
         <v>45422</v>
       </c>
@@ -47331,7 +47341,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A314" s="3">
         <v>45430</v>
       </c>
@@ -47385,7 +47395,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A316" s="3">
         <v>45432</v>
       </c>
@@ -47412,7 +47422,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A317" s="3">
         <v>45432</v>
       </c>
@@ -47466,7 +47476,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A319" s="3">
         <v>45434</v>
       </c>
@@ -47547,7 +47557,7 @@
         <v>1022.25</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A322" s="3">
         <v>45443</v>
       </c>
@@ -47601,7 +47611,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A324" s="3">
         <v>45443</v>
       </c>
@@ -47628,7 +47638,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A325" s="3">
         <v>45443</v>
       </c>
@@ -47709,7 +47719,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A328" s="3">
         <v>45446</v>
       </c>
@@ -47763,7 +47773,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A330" s="3">
         <v>45454</v>
       </c>
@@ -47791,7 +47801,7 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A331" s="3">
         <v>45458</v>
       </c>
@@ -47845,7 +47855,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A333" s="3">
         <v>45459</v>
       </c>
@@ -47899,7 +47909,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A335" s="3">
         <v>45461</v>
       </c>
@@ -47953,7 +47963,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A337" s="3">
         <v>45465</v>
       </c>
@@ -47980,7 +47990,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A338" s="3">
         <v>45465</v>
       </c>
@@ -48034,7 +48044,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A340" s="3">
         <v>45472</v>
       </c>
@@ -48088,7 +48098,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A342" s="3">
         <v>45473</v>
       </c>
@@ -48115,7 +48125,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A343" s="3">
         <v>45473</v>
       </c>
@@ -48142,7 +48152,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A344" s="3">
         <v>45473</v>
       </c>
@@ -48170,7 +48180,7 @@
         <v>2940</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A345" s="3">
         <v>45473</v>
       </c>
@@ -48197,7 +48207,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A346" s="3">
         <v>45473</v>
       </c>
@@ -48224,7 +48234,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A347" s="3">
         <v>45473</v>
       </c>
@@ -48251,7 +48261,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A348" s="3">
         <v>45473</v>
       </c>
@@ -48413,7 +48423,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A354" s="3">
         <v>45488</v>
       </c>
@@ -48521,7 +48531,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A358" s="3">
         <v>45498</v>
       </c>
@@ -48548,7 +48558,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A359" s="3">
         <v>45498</v>
       </c>
@@ -48926,7 +48936,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A373" s="3">
         <v>45520</v>
       </c>
@@ -49061,7 +49071,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A378" s="3">
         <v>45534</v>
       </c>
@@ -49142,7 +49152,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A381" s="3">
         <v>45535</v>
       </c>
@@ -49223,7 +49233,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A384" s="3">
         <v>45535</v>
       </c>
@@ -49250,7 +49260,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A385" s="3">
         <v>45535</v>
       </c>
@@ -49358,7 +49368,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A389" s="3">
         <v>45541</v>
       </c>
@@ -49438,7 +49448,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A392" s="3">
         <v>45552</v>
       </c>
@@ -49898,7 +49908,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A409" s="3">
         <v>45580</v>
       </c>
@@ -50277,7 +50287,7 @@
         <v>1773.35</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A423" s="3">
         <v>45598</v>
       </c>
@@ -50358,7 +50368,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A426" s="3">
         <v>45604</v>
       </c>
@@ -50546,7 +50556,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A433" s="3">
         <v>45612</v>
       </c>
@@ -50708,7 +50718,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A439" s="3">
         <v>45626</v>
       </c>
@@ -50816,7 +50826,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A443" s="3">
         <v>45626</v>
       </c>
@@ -50843,7 +50853,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A444" s="3">
         <v>45626</v>
       </c>
@@ -51059,7 +51069,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="452" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A452" s="3">
         <v>45637</v>
       </c>
@@ -51330,7 +51340,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="462" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="462" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A462" s="3">
         <v>45649</v>
       </c>
@@ -51679,7 +51689,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="475" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A475" s="3">
         <v>45665</v>
       </c>
@@ -51706,7 +51716,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A476" s="3">
         <v>45670</v>
       </c>
@@ -51867,7 +51877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="482" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A482" s="3">
         <v>45677</v>
       </c>
@@ -51948,7 +51958,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A485" s="3">
         <v>45679</v>
       </c>
@@ -52434,7 +52444,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="503" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A503" s="3">
         <v>45704</v>
       </c>
@@ -52893,7 +52903,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="520" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A520" s="3">
         <v>45717</v>
       </c>
@@ -53000,7 +53010,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="524" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="524" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A524" s="3">
         <v>45732</v>
       </c>
@@ -53108,7 +53118,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="528" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="528" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A528" s="3">
         <v>45739</v>
       </c>
@@ -53514,7 +53524,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="543" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="543" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A543" s="3">
         <v>45763</v>
       </c>
@@ -53893,7 +53903,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="557" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="557" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A557" s="3">
         <v>45782</v>
       </c>
@@ -54379,7 +54389,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="575" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="575" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A575" s="3">
         <v>45808</v>
       </c>
@@ -57359,7 +57369,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="685" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="685" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A685" s="3">
         <v>45947</v>
       </c>
@@ -58250,7 +58260,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="718" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="718" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A718" s="3">
         <v>45991</v>
       </c>
@@ -58574,7 +58584,7 @@
         <v>3302.96</v>
       </c>
     </row>
-    <row r="730" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="730" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A730" s="3"/>
       <c r="G730" s="23"/>
       <c r="H730" s="4">
@@ -58582,7 +58592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="731" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="731" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A731" s="3"/>
       <c r="G731" s="23"/>
       <c r="H731" s="4">
@@ -58590,7 +58600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="732" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="732" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A732" s="3"/>
       <c r="G732" s="23"/>
       <c r="H732" s="4">
@@ -58598,7 +58608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="733" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="733" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A733" s="3"/>
       <c r="G733" s="23"/>
       <c r="H733" s="4">
@@ -58606,7 +58616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="734" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="734" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A734" s="3"/>
       <c r="G734" s="23"/>
       <c r="H734" s="4">
@@ -58614,7 +58624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="735" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="735" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A735" s="3"/>
       <c r="G735" s="23"/>
       <c r="H735" s="4">
@@ -58622,7 +58632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="736" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="736" spans="1:8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A736" s="3"/>
       <c r="G736" s="23"/>
       <c r="H736" s="4">
@@ -59790,7 +59800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195A0105-3A59-49D8-BD5A-3DA537A00814}">
   <dimension ref="A1:BB45"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Producción OK 040226 - Backup de respaldo previo a implementacion de alertas y notificaciones por correo
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Gastos Socios Symbiot.xlsx
+++ b/Gastos Socios Symbiot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\symbiot\symbiot_finance_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4E6BAA-7092-436E-8A08-672FA196458A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB80A3D-B3C6-491A-A734-8E068FDC0F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" tabRatio="773" activeTab="2" xr2:uid="{9089598D-A971-4695-A3E9-38E00D99589C}"/>
   </bookViews>
@@ -2807,149 +2807,6 @@
   </cellStyles>
   <dxfs count="151">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -3200,7 +3057,29 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3208,7 +3087,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3216,7 +3094,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3224,7 +3101,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3232,7 +3108,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3240,7 +3115,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3248,7 +3122,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3256,11 +3129,62 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3274,7 +3198,107 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
@@ -3285,55 +3309,16 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3356,6 +3341,21 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -18215,17 +18215,17 @@
     <dataField name="Sum of Total" fld="47" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="60">
+    <format dxfId="19">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="18">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
@@ -18367,13 +18367,13 @@
     <dataField name="Suma de Noviembre3" fld="45" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="64">
+    <format dxfId="23">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="21">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2" selected="0">
@@ -18383,7 +18383,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2">
@@ -18543,13 +18543,13 @@
     <dataField name="Suma de Noviembre3" fld="45" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="68">
+    <format dxfId="27">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="67">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="66">
+    <format dxfId="25">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2" selected="0">
@@ -18559,7 +18559,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2">
@@ -18704,13 +18704,13 @@
     <dataField name="Count of Alumno" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="72">
+    <format dxfId="31">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="30">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="29">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2" selected="0">
@@ -18720,7 +18720,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="2">
@@ -18870,13 +18870,13 @@
     <dataField name="Count of Estatus" fld="15" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="75">
+    <format dxfId="34">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="33">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="32">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="15" count="0"/>
@@ -19033,7 +19033,7 @@
     <dataField name="Count of Alumno" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="80">
+    <format dxfId="39">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="7">
@@ -19048,24 +19048,24 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="36">
       <pivotArea field="8" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="35">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -19506,61 +19506,61 @@
     <dataField name="Suma de Total" fld="6" baseField="0" baseItem="0" numFmtId="8"/>
   </dataFields>
   <formats count="16">
-    <format dxfId="56">
+    <format dxfId="15">
       <pivotArea field="2" outline="0" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="13">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="12">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="11">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="8">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="5">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="3">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="1">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1" selected="0">
@@ -19569,7 +19569,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="2" count="1">
@@ -20198,7 +20198,7 @@
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0" numFmtId="168"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="57">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -20253,131 +20253,137 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9B0D3573-E4D3-46D4-8941-9E5BFEB561B5}" name="Table14" displayName="Table14" ref="A1:AX121" totalsRowCount="1" headerRowDxfId="134">
-  <autoFilter ref="A1:AX120" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}"/>
+  <autoFilter ref="A1:AX120" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}">
+    <filterColumn colId="47">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX120">
     <sortCondition ref="B1:B120"/>
   </sortState>
   <tableColumns count="50">
-    <tableColumn id="1" xr3:uid="{22FE3325-3F0C-4FF9-B9FF-47A645BFCF04}" name="Num Alumno" dataDxfId="133" totalsRowDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{22FE3325-3F0C-4FF9-B9FF-47A645BFCF04}" name="Num Alumno" dataDxfId="133" totalsRowDxfId="132"/>
     <tableColumn id="2" xr3:uid="{381104ED-278D-448C-85FC-4A7E3AF3DC05}" name="Alumno"/>
-    <tableColumn id="10" xr3:uid="{E92BE7EA-EBB2-4A0C-96E2-0DBE48306F37}" name="Edad" dataDxfId="132" totalsRowDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{E92BE7EA-EBB2-4A0C-96E2-0DBE48306F37}" name="Edad" dataDxfId="131" totalsRowDxfId="130"/>
     <tableColumn id="3" xr3:uid="{A82F4F10-B150-43BC-AA9C-55D716B38D02}" name="Maestro"/>
-    <tableColumn id="9" xr3:uid="{587C9B83-F274-4FFB-8C7B-8E74CB25FF97}" name="Fecha de inscripción" dataDxfId="131" totalsRowDxfId="38"/>
-    <tableColumn id="11" xr3:uid="{0CCD438F-3692-470C-A478-28A1B4CE6DB7}" name="Fecha de pago" dataDxfId="130" totalsRowDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{587C9B83-F274-4FFB-8C7B-8E74CB25FF97}" name="Fecha de inscripción" dataDxfId="129" totalsRowDxfId="128"/>
+    <tableColumn id="11" xr3:uid="{0CCD438F-3692-470C-A478-28A1B4CE6DB7}" name="Fecha de pago" dataDxfId="127" totalsRowDxfId="126"/>
     <tableColumn id="12" xr3:uid="{C193D3F5-A6B5-415B-B7B0-7A3907E31527}" name="Promocion"/>
     <tableColumn id="8" xr3:uid="{BA7E9AC7-2995-42D9-8226-9BC64D135045}" name="Clase"/>
-    <tableColumn id="13" xr3:uid="{59A71299-E821-4D87-8D12-806FC34A1078}" name="Tipo" dataDxfId="129" totalsRowDxfId="36"/>
+    <tableColumn id="13" xr3:uid="{59A71299-E821-4D87-8D12-806FC34A1078}" name="Tipo" dataDxfId="125" totalsRowDxfId="124"/>
     <tableColumn id="14" xr3:uid="{C964548A-02EC-43E6-8589-9FE5EC5BCEFC}" name="Horario"/>
-    <tableColumn id="4" xr3:uid="{DBC42755-FCEC-4041-A87A-25A120DAACEB}" name="Forma de Pago" dataDxfId="128" totalsRowDxfId="35"/>
-    <tableColumn id="32" xr3:uid="{12E66F8C-E7D1-42D2-963B-FCFD6BA6427F}" name="Domicilado" dataDxfId="127" totalsRowDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{63649793-4429-42F0-AC13-D5B992DC1A9D}" name="Cantidad" dataDxfId="126" totalsRowDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{908CCE59-350B-4302-8336-6728C7319715}" name="Precio x unidad" dataDxfId="125" totalsRowDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{DBC42755-FCEC-4041-A87A-25A120DAACEB}" name="Forma de Pago" dataDxfId="123" totalsRowDxfId="122"/>
+    <tableColumn id="32" xr3:uid="{12E66F8C-E7D1-42D2-963B-FCFD6BA6427F}" name="Domicilado" dataDxfId="121" totalsRowDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{63649793-4429-42F0-AC13-D5B992DC1A9D}" name="Cantidad" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="6" xr3:uid="{908CCE59-350B-4302-8336-6728C7319715}" name="Precio x unidad" dataDxfId="117" totalsRowDxfId="116"/>
     <tableColumn id="15" xr3:uid="{EDE007B4-CFFC-4066-9B63-8AA0D38E36FF}" name="Domicilado2"/>
     <tableColumn id="16" xr3:uid="{619A5E6C-0A6A-4535-9EE8-CEECC82883F2}" name="Estatus"/>
-    <tableColumn id="28" xr3:uid="{0B8D5572-80AA-4526-B946-CED9E498BEA9}" name="Tipo de Clase" dataDxfId="124">
+    <tableColumn id="28" xr3:uid="{0B8D5572-80AA-4526-B946-CED9E498BEA9}" name="Tipo de Clase" dataDxfId="115">
       <calculatedColumnFormula>_xlfn.CONCAT(Table14[[#This Row],[Clase]]," ",Table14[[#This Row],[Tipo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{6CE68872-BD3E-423E-A8F4-68534FD74DF8}" name="Julio" totalsRowFunction="custom" totalsRowDxfId="31">
+    <tableColumn id="17" xr3:uid="{6CE68872-BD3E-423E-A8F4-68534FD74DF8}" name="Julio" totalsRowFunction="custom" totalsRowDxfId="114">
       <totalsRowFormula>SUM(R2:R120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{F06B3061-C34F-4ADC-8B79-AF6755CA94B1}" name="Agosto" totalsRowFunction="custom" dataDxfId="123" totalsRowDxfId="30">
+    <tableColumn id="18" xr3:uid="{F06B3061-C34F-4ADC-8B79-AF6755CA94B1}" name="Agosto" totalsRowFunction="custom" dataDxfId="113" totalsRowDxfId="112">
       <totalsRowFormula>SUM(S2:S120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{4EAAF530-4B11-48C0-A9B7-CAA4E0AA70F2}" name="Septiembre" totalsRowFunction="custom" dataDxfId="122" totalsRowDxfId="29">
+    <tableColumn id="19" xr3:uid="{4EAAF530-4B11-48C0-A9B7-CAA4E0AA70F2}" name="Septiembre" totalsRowFunction="custom" dataDxfId="111" totalsRowDxfId="110">
       <totalsRowFormula>SUM(T2:T120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{46B2AE54-BE68-48F8-9798-57D10A97EF39}" name="Octubre" totalsRowFunction="custom" dataDxfId="121" totalsRowDxfId="28">
+    <tableColumn id="20" xr3:uid="{46B2AE54-BE68-48F8-9798-57D10A97EF39}" name="Octubre" totalsRowFunction="custom" dataDxfId="109" totalsRowDxfId="108">
       <totalsRowFormula>SUM(U2:U120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{DCAABE8E-47E1-410B-B7AC-BE18E0142970}" name="Noviembre" totalsRowFunction="custom" dataDxfId="120" totalsRowDxfId="27">
+    <tableColumn id="21" xr3:uid="{DCAABE8E-47E1-410B-B7AC-BE18E0142970}" name="Noviembre" totalsRowFunction="custom" dataDxfId="107" totalsRowDxfId="106">
       <totalsRowFormula>SUM(V2:V120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{981A4256-C0F9-4DAE-980D-7147BEB52904}" name="Diciembre" totalsRowFunction="custom" dataDxfId="119" totalsRowDxfId="26">
+    <tableColumn id="22" xr3:uid="{981A4256-C0F9-4DAE-980D-7147BEB52904}" name="Diciembre" totalsRowFunction="custom" dataDxfId="105" totalsRowDxfId="104">
       <totalsRowFormula>SUM(W2:W120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{6BA15BD9-3A29-48F7-B5EB-6DB2FC89EB39}" name="Enero" totalsRowFunction="custom" dataDxfId="118" totalsRowDxfId="25">
+    <tableColumn id="24" xr3:uid="{6BA15BD9-3A29-48F7-B5EB-6DB2FC89EB39}" name="Enero" totalsRowFunction="custom" dataDxfId="103" totalsRowDxfId="102">
       <totalsRowFormula>SUM(X2:X120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{8E9C40ED-116E-4F34-8AA5-8D33D0E66CDF}" name="Febrero" totalsRowFunction="custom" dataDxfId="117" totalsRowDxfId="24">
+    <tableColumn id="23" xr3:uid="{8E9C40ED-116E-4F34-8AA5-8D33D0E66CDF}" name="Febrero" totalsRowFunction="custom" dataDxfId="101" totalsRowDxfId="100">
       <totalsRowFormula>SUM(Y2:Y120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{6B1BD976-8574-490D-B67F-A78939C42A50}" name="Marzo" totalsRowFunction="custom" dataDxfId="116" totalsRowDxfId="23">
+    <tableColumn id="26" xr3:uid="{6B1BD976-8574-490D-B67F-A78939C42A50}" name="Marzo" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="98">
       <totalsRowFormula>SUM(Z2:Z120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{F952A291-66AC-49B4-B371-67AA03BF30EF}" name="Abril" totalsRowFunction="custom" dataDxfId="115" totalsRowDxfId="22">
+    <tableColumn id="27" xr3:uid="{F952A291-66AC-49B4-B371-67AA03BF30EF}" name="Abril" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="96">
       <totalsRowFormula>SUM(AA2:AA120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{2E4828CA-68D9-474A-81C5-FFF34121BD95}" name="Mayo" totalsRowFunction="custom" dataDxfId="114" totalsRowDxfId="21">
+    <tableColumn id="25" xr3:uid="{2E4828CA-68D9-474A-81C5-FFF34121BD95}" name="Mayo" totalsRowFunction="custom" dataDxfId="95" totalsRowDxfId="94">
       <totalsRowFormula>SUM(AB2:AB120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{E796EFC8-A70B-415C-BDA5-CE0977C1A2EE}" name="Junio" totalsRowFunction="custom" dataDxfId="113" totalsRowDxfId="20">
+    <tableColumn id="31" xr3:uid="{E796EFC8-A70B-415C-BDA5-CE0977C1A2EE}" name="Junio" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="92">
       <totalsRowFormula>SUM(AC2:AC120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{28D759F4-8442-4888-9566-C336035DFDC1}" name="Julio2" totalsRowFunction="custom" dataDxfId="112" totalsRowDxfId="19">
+    <tableColumn id="30" xr3:uid="{28D759F4-8442-4888-9566-C336035DFDC1}" name="Julio2" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="90">
       <totalsRowFormula>SUM(AD2:AD120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{AD78B7A4-514A-4D16-8EB3-9D2808950D45}" name="Agosto2" totalsRowFunction="custom" dataDxfId="111" totalsRowDxfId="18">
+    <tableColumn id="29" xr3:uid="{AD78B7A4-514A-4D16-8EB3-9D2808950D45}" name="Agosto2" totalsRowFunction="custom" dataDxfId="89" totalsRowDxfId="88">
       <totalsRowFormula>SUM(AE2:AE120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{A91A2628-B7DF-47B2-8012-5A1394E22930}" name="Septiembre2" totalsRowFunction="custom" dataDxfId="110" totalsRowDxfId="17">
+    <tableColumn id="33" xr3:uid="{A91A2628-B7DF-47B2-8012-5A1394E22930}" name="Septiembre2" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="86">
       <totalsRowFormula>SUM(AF2:AF120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{261370ED-3AFA-47F0-B6C4-7C7FB0348ED8}" name="Octubre2" totalsRowFunction="custom" dataDxfId="109" totalsRowDxfId="16">
+    <tableColumn id="34" xr3:uid="{261370ED-3AFA-47F0-B6C4-7C7FB0348ED8}" name="Octubre2" totalsRowFunction="custom" dataDxfId="85" totalsRowDxfId="84">
       <totalsRowFormula>SUM(AG2:AG120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{BBFF8603-7E74-40F7-81A8-7A8265011B1C}" name="Noviembre2" totalsRowFunction="custom" dataDxfId="108" totalsRowDxfId="15">
+    <tableColumn id="35" xr3:uid="{BBFF8603-7E74-40F7-81A8-7A8265011B1C}" name="Noviembre2" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="82">
       <totalsRowFormula>SUM(AH2:AH120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{69917871-8EB9-454A-B400-8684D1C21365}" name="Diciembre3" totalsRowFunction="custom" dataDxfId="107" totalsRowDxfId="14">
+    <tableColumn id="39" xr3:uid="{69917871-8EB9-454A-B400-8684D1C21365}" name="Diciembre3" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="80">
       <totalsRowFormula>SUM(AI2:AI120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{E488B402-03D6-4BD8-9D03-B3A9E9BCE9A5}" name="Enero2" totalsRowFunction="custom" dataDxfId="106" totalsRowDxfId="13">
+    <tableColumn id="38" xr3:uid="{E488B402-03D6-4BD8-9D03-B3A9E9BCE9A5}" name="Enero2" totalsRowFunction="custom" dataDxfId="79" totalsRowDxfId="78">
       <totalsRowFormula>SUM(AJ2:AJ120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{FECEF4BB-C58F-41A8-8300-FDAE1681476D}" name="Febrero2" totalsRowFunction="custom" dataDxfId="105" totalsRowDxfId="12">
+    <tableColumn id="37" xr3:uid="{FECEF4BB-C58F-41A8-8300-FDAE1681476D}" name="Febrero2" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
       <totalsRowFormula>SUM(AK2:AK120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{38114AE3-C756-41D4-8042-7F4EE908E86C}" name="Marzo2" totalsRowFunction="custom" dataDxfId="104" totalsRowDxfId="11">
+    <tableColumn id="40" xr3:uid="{38114AE3-C756-41D4-8042-7F4EE908E86C}" name="Marzo2" totalsRowFunction="custom" dataDxfId="75" totalsRowDxfId="74">
       <totalsRowFormula>SUM(AL2:AL120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{CAD53A45-5676-468A-8720-9FC1DC6DE69A}" name="Abril2" totalsRowFunction="custom" dataDxfId="103" totalsRowDxfId="10">
+    <tableColumn id="42" xr3:uid="{CAD53A45-5676-468A-8720-9FC1DC6DE69A}" name="Abril2" totalsRowFunction="custom" dataDxfId="73" totalsRowDxfId="72">
       <totalsRowFormula>SUM(AM2:AM120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{F3CE6FAF-D6F8-4EA3-A043-2AF18436CDEA}" name="Mayo2" totalsRowFunction="custom" dataDxfId="102" totalsRowDxfId="9">
+    <tableColumn id="41" xr3:uid="{F3CE6FAF-D6F8-4EA3-A043-2AF18436CDEA}" name="Mayo2" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="70">
       <totalsRowFormula>SUM(AN2:AN120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{F804E5FB-A23F-4F9E-8E45-BB961E0446FB}" name="Junio2" totalsRowFunction="custom" dataDxfId="101" totalsRowDxfId="8">
+    <tableColumn id="45" xr3:uid="{F804E5FB-A23F-4F9E-8E45-BB961E0446FB}" name="Junio2" totalsRowFunction="custom" dataDxfId="69" totalsRowDxfId="68">
       <totalsRowFormula>SUM(AO2:AO120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{855B17F7-EF24-4B21-AF6D-46A6497B9136}" name="Julio3" totalsRowFunction="custom" dataDxfId="100" totalsRowDxfId="7">
+    <tableColumn id="46" xr3:uid="{855B17F7-EF24-4B21-AF6D-46A6497B9136}" name="Julio3" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
       <totalsRowFormula>SUM(AP2:AP120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{C61B0969-E8FF-421E-958A-3C8E2F41D676}" name="Agosto3" totalsRowFunction="custom" dataDxfId="99" totalsRowDxfId="6">
+    <tableColumn id="44" xr3:uid="{C61B0969-E8FF-421E-958A-3C8E2F41D676}" name="Agosto3" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="64">
       <totalsRowFormula>SUM(AQ2:AQ120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{7EFA7755-CAAA-49E1-B0AA-4EFBDE1A47FD}" name="Septiembre3" totalsRowFunction="custom" dataDxfId="98" totalsRowDxfId="5">
+    <tableColumn id="36" xr3:uid="{7EFA7755-CAAA-49E1-B0AA-4EFBDE1A47FD}" name="Septiembre3" totalsRowFunction="custom" dataDxfId="63" totalsRowDxfId="62">
       <totalsRowFormula>SUM(AR2:AR120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{F287CABE-D5B2-457A-999C-739B201CDF8E}" name="Octubre3" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="4">
+    <tableColumn id="49" xr3:uid="{F287CABE-D5B2-457A-999C-739B201CDF8E}" name="Octubre3" totalsRowFunction="custom" dataDxfId="61" totalsRowDxfId="60">
       <totalsRowFormula>SUM(AS2:AS120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{6C5A7346-2A0E-4155-BF17-CD5908A2FC24}" name="Noviembre3" totalsRowFunction="custom" dataDxfId="96" totalsRowDxfId="3">
+    <tableColumn id="48" xr3:uid="{6C5A7346-2A0E-4155-BF17-CD5908A2FC24}" name="Noviembre3" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
       <totalsRowFormula>SUM(AT2:AT120)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="47" xr3:uid="{A0F0DEC6-5B71-42DE-A3B1-3D5E32C0CAC0}" name="Diciembre2" dataDxfId="95" totalsRowDxfId="2"/>
-    <tableColumn id="50" xr3:uid="{FF6F6226-F427-490D-A2AA-5D786EA18AC0}" name="Enero3" dataDxfId="94" totalsRowDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{4D4FC95B-B09A-4BC5-A65D-05D6A8A0C3FE}" name="Total" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="0">
+    <tableColumn id="47" xr3:uid="{A0F0DEC6-5B71-42DE-A3B1-3D5E32C0CAC0}" name="Diciembre2" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="50" xr3:uid="{FF6F6226-F427-490D-A2AA-5D786EA18AC0}" name="Enero3" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{4D4FC95B-B09A-4BC5-A65D-05D6A8A0C3FE}" name="Total" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula>SUM(Table14[[#This Row],[Julio]:[Diciembre2]])</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table14[Total])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{35D56830-A1AF-4602-836F-A57DCC0B92C6}" name="Observaciones" dataDxfId="92"/>
+    <tableColumn id="43" xr3:uid="{35D56830-A1AF-4602-836F-A57DCC0B92C6}" name="Observaciones" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}" name="Table1" displayName="Table1" ref="A1:H737" totalsRowCount="1" headerRowDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}" name="Table1" displayName="Table1" ref="A1:H737" totalsRowCount="1" headerRowDxfId="50">
   <autoFilter ref="A1:H736" xr:uid="{BFA399A6-7457-466A-A8E1-0C581281E875}">
     <filterColumn colId="2">
       <filters>
@@ -20389,14 +20395,14 @@
     <sortCondition ref="A1:A736"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E1AD0ECF-72E7-4EE2-B6E5-D7A5D15CAB4D}" name="Fecha" totalsRowLabel="Total" dataDxfId="90" totalsRowDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{E1AD0ECF-72E7-4EE2-B6E5-D7A5D15CAB4D}" name="Fecha" totalsRowLabel="Total" dataDxfId="49" totalsRowDxfId="48"/>
     <tableColumn id="2" xr3:uid="{255E6142-348E-4056-847C-FC1B935C536B}" name="Concepto"/>
     <tableColumn id="3" xr3:uid="{6DF4309C-0761-4ABE-8464-F84E5EB9223A}" name="Socio"/>
     <tableColumn id="8" xr3:uid="{E8D90A93-C13C-45B4-99F6-B8214C67B72B}" name="Transacción ID"/>
-    <tableColumn id="4" xr3:uid="{0DD5A2EC-CF0D-4EA8-B7EA-217AC263A04D}" name="Forma de Pago" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="5" xr3:uid="{4C5448DE-9D16-4C9C-8CE2-7246FBA56126}" name="Cantidad" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="6" xr3:uid="{F298497C-54D4-4EAC-AEFF-A51217F4A6CC}" name="Precio x unidad" dataDxfId="84" totalsRowDxfId="83"/>
-    <tableColumn id="7" xr3:uid="{9B6E0B5E-4AFE-4DF6-BE01-3F529965C090}" name="Total" totalsRowFunction="custom" dataDxfId="82" totalsRowDxfId="81">
+    <tableColumn id="4" xr3:uid="{0DD5A2EC-CF0D-4EA8-B7EA-217AC263A04D}" name="Forma de Pago" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{4C5448DE-9D16-4C9C-8CE2-7246FBA56126}" name="Cantidad" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{F298497C-54D4-4EAC-AEFF-A51217F4A6CC}" name="Precio x unidad" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{9B6E0B5E-4AFE-4DF6-BE01-3F529965C090}" name="Total" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <totalsRowFormula>SUM(Table1[Total])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -22452,10 +22458,10 @@
   <dimension ref="A1:AZ127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F49" sqref="F49"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -22660,7 +22666,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="2" spans="1:50" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:50" s="31" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" s="53">
         <v>88</v>
       </c>
@@ -22960,7 +22966,7 @@
       </c>
       <c r="AX3" s="23"/>
     </row>
-    <row r="4" spans="1:50" s="27" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:50" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" s="64">
         <v>87</v>
       </c>
@@ -23408,7 +23414,7 @@
       </c>
       <c r="AX6" s="23"/>
     </row>
-    <row r="7" spans="1:50" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:50" s="31" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" s="64">
         <v>2</v>
       </c>
@@ -23704,7 +23710,7 @@
       </c>
       <c r="AX8" s="23"/>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" s="64">
         <v>33</v>
       </c>
@@ -24006,7 +24012,7 @@
       </c>
       <c r="AX10" s="23"/>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" s="64">
         <v>17</v>
       </c>
@@ -24913,7 +24919,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" s="64">
         <v>76</v>
       </c>
@@ -25059,7 +25065,7 @@
       </c>
       <c r="AX17" s="30"/>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A18" s="64">
         <v>95</v>
       </c>
@@ -25205,7 +25211,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" s="64">
         <v>11</v>
       </c>
@@ -25647,7 +25653,7 @@
       </c>
       <c r="AX21" s="41"/>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" s="64">
         <v>53</v>
       </c>
@@ -25795,7 +25801,7 @@
       </c>
       <c r="AX22" s="23"/>
     </row>
-    <row r="23" spans="1:50" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:50" s="31" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="64">
         <v>69</v>
       </c>
@@ -26094,7 +26100,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" s="64">
         <v>57</v>
       </c>
@@ -26240,7 +26246,7 @@
       </c>
       <c r="AX25" s="23"/>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A26" s="64">
         <v>20</v>
       </c>
@@ -26386,7 +26392,7 @@
       </c>
       <c r="AX26" s="23"/>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" s="64">
         <v>21</v>
       </c>
@@ -26679,7 +26685,7 @@
       </c>
       <c r="AX28" s="23"/>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A29" s="64">
         <v>68</v>
       </c>
@@ -27118,7 +27124,7 @@
       </c>
       <c r="AX31" s="23"/>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" s="64">
         <v>45</v>
       </c>
@@ -27269,7 +27275,7 @@
       </c>
       <c r="AX32" s="23"/>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A33" s="64">
         <v>41</v>
       </c>
@@ -27419,7 +27425,7 @@
       </c>
       <c r="AX33" s="23"/>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A34" s="64">
         <v>84</v>
       </c>
@@ -28164,7 +28170,7 @@
       </c>
       <c r="AX38" s="23"/>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" s="64">
         <v>9</v>
       </c>
@@ -28312,7 +28318,7 @@
       </c>
       <c r="AX39" s="23"/>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" s="64">
         <v>10</v>
       </c>
@@ -28464,7 +28470,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A41" s="64">
         <v>27</v>
       </c>
@@ -28614,7 +28620,7 @@
       </c>
       <c r="AX41" s="23"/>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A42" s="64">
         <v>92</v>
       </c>
@@ -29208,7 +29214,7 @@
       </c>
       <c r="AX45" s="23"/>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:52" hidden="1" x14ac:dyDescent="0.4">
       <c r="A46" s="64">
         <v>67</v>
       </c>
@@ -29938,7 +29944,7 @@
       </c>
       <c r="AX50" s="23"/>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A51" s="64">
         <v>1</v>
       </c>
@@ -30084,7 +30090,7 @@
       </c>
       <c r="AX51" s="30"/>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A52" s="64">
         <v>80</v>
       </c>
@@ -30230,7 +30236,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A53" s="64">
         <v>64</v>
       </c>
@@ -30372,7 +30378,7 @@
       </c>
       <c r="AX53" s="23"/>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A54" s="64">
         <v>14</v>
       </c>
@@ -30665,7 +30671,7 @@
       </c>
       <c r="AX55" s="23"/>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A56" s="64">
         <v>39</v>
       </c>
@@ -30816,7 +30822,7 @@
       </c>
       <c r="AX56" s="23"/>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A57" s="64">
         <v>40</v>
       </c>
@@ -30967,7 +30973,7 @@
       </c>
       <c r="AX57" s="23"/>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A58" s="64">
         <v>13</v>
       </c>
@@ -31115,7 +31121,7 @@
       </c>
       <c r="AX58" s="30"/>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A59" s="64">
         <v>48</v>
       </c>
@@ -31265,7 +31271,7 @@
       </c>
       <c r="AX59" s="23"/>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A60" s="64">
         <v>6</v>
       </c>
@@ -31411,7 +31417,7 @@
       </c>
       <c r="AX60" s="23"/>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A61" s="64">
         <v>3</v>
       </c>
@@ -32148,7 +32154,7 @@
       </c>
       <c r="AX65" s="23"/>
     </row>
-    <row r="66" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A66" s="64">
         <v>15</v>
       </c>
@@ -32298,7 +32304,7 @@
       </c>
       <c r="AX66" s="23"/>
     </row>
-    <row r="67" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A67" s="64">
         <v>49</v>
       </c>
@@ -32601,7 +32607,7 @@
       </c>
       <c r="AX68" s="23"/>
     </row>
-    <row r="69" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A69" s="64">
         <v>22</v>
       </c>
@@ -32747,7 +32753,7 @@
       </c>
       <c r="AX69" s="23"/>
     </row>
-    <row r="70" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A70" s="64">
         <v>23</v>
       </c>
@@ -33045,7 +33051,7 @@
       </c>
       <c r="AX71" s="23"/>
     </row>
-    <row r="72" spans="1:50" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:50" s="31" customFormat="1" hidden="1" x14ac:dyDescent="0.4">
       <c r="A72" s="64">
         <v>37</v>
       </c>
@@ -33195,7 +33201,7 @@
       </c>
       <c r="AX72" s="23"/>
     </row>
-    <row r="73" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A73" s="64">
         <v>5</v>
       </c>
@@ -33345,7 +33351,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="74" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A74" s="64">
         <v>46</v>
       </c>
@@ -33495,7 +33501,7 @@
       </c>
       <c r="AX74" s="23"/>
     </row>
-    <row r="75" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A75" s="64">
         <v>51</v>
       </c>
@@ -33643,7 +33649,7 @@
       </c>
       <c r="AX75" s="23"/>
     </row>
-    <row r="76" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A76" s="64">
         <v>52</v>
       </c>
@@ -33941,7 +33947,7 @@
       </c>
       <c r="AX77" s="23"/>
     </row>
-    <row r="78" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A78" s="64">
         <v>86</v>
       </c>
@@ -34085,7 +34091,7 @@
       </c>
       <c r="AX78" s="23"/>
     </row>
-    <row r="79" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A79" s="64">
         <v>25</v>
       </c>
@@ -34387,7 +34393,7 @@
       </c>
       <c r="AX80" s="23"/>
     </row>
-    <row r="81" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A81" s="64">
         <v>4</v>
       </c>
@@ -34533,7 +34539,7 @@
       </c>
       <c r="AX81" s="30"/>
     </row>
-    <row r="82" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A82" s="64">
         <v>78</v>
       </c>
@@ -35283,7 +35289,7 @@
       </c>
       <c r="AX86" s="23"/>
     </row>
-    <row r="87" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A87" s="64">
         <v>18</v>
       </c>
@@ -35581,7 +35587,7 @@
       </c>
       <c r="AX88" s="23"/>
     </row>
-    <row r="89" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A89" s="64">
         <v>101</v>
       </c>
@@ -35725,7 +35731,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="90" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A90" s="64">
         <v>50</v>
       </c>
@@ -35873,7 +35879,7 @@
       </c>
       <c r="AX90" s="23"/>
     </row>
-    <row r="91" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A91" s="64">
         <v>19</v>
       </c>
@@ -36324,7 +36330,7 @@
       </c>
       <c r="AX93" s="23"/>
     </row>
-    <row r="94" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A94" s="64">
         <v>60</v>
       </c>
@@ -36619,7 +36625,7 @@
       </c>
       <c r="AX95" s="23"/>
     </row>
-    <row r="96" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A96" s="64">
         <v>35</v>
       </c>
@@ -36769,7 +36775,7 @@
       </c>
       <c r="AX96" s="23"/>
     </row>
-    <row r="97" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A97" s="64">
         <v>36</v>
       </c>
@@ -37062,7 +37068,7 @@
       </c>
       <c r="AX98" s="23"/>
     </row>
-    <row r="99" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A99" s="64">
         <v>30</v>
       </c>
@@ -37359,7 +37365,7 @@
       </c>
       <c r="AX100" s="23"/>
     </row>
-    <row r="101" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A101" s="64">
         <v>81</v>
       </c>
@@ -37505,7 +37511,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="102" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A102" s="64">
         <v>82</v>
       </c>
@@ -37801,7 +37807,7 @@
       </c>
       <c r="AX103" s="23"/>
     </row>
-    <row r="104" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A104" s="64">
         <v>79</v>
       </c>
@@ -38240,7 +38246,7 @@
       </c>
       <c r="AX106" s="23"/>
     </row>
-    <row r="107" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A107" s="64">
         <v>47</v>
       </c>
@@ -38539,7 +38545,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="109" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A109" s="64">
         <v>31</v>
       </c>
@@ -38687,7 +38693,7 @@
       </c>
       <c r="AX109" s="23"/>
     </row>
-    <row r="110" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A110" s="64">
         <v>32</v>
       </c>
@@ -39522,7 +39528,7 @@
       </c>
       <c r="AX118" s="23"/>
     </row>
-    <row r="119" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A119" s="22"/>
       <c r="N119" s="23"/>
       <c r="Q119" t="str">
@@ -39565,7 +39571,7 @@
       </c>
       <c r="AX119" s="23"/>
     </row>
-    <row r="120" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:50" hidden="1" x14ac:dyDescent="0.4">
       <c r="A120" s="22"/>
       <c r="N120" s="23"/>
       <c r="Q120" t="str">
@@ -39760,7 +39766,7 @@
   <dimension ref="A1:L737"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A676" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A698" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I200" sqref="I200"/>
     </sheetView>
   </sheetViews>

</xml_diff>